<commit_message>
find min and update bert
</commit_message>
<xml_diff>
--- a/Output/Bert_output.xlsx
+++ b/Output/Bert_output.xlsx
@@ -773,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8841983270645142</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.8360749292373657</v>
+        <v>0.7861067056655884</v>
       </c>
       <c r="D2">
-        <v>0.8260028314590454</v>
+        <v>0.7479889392852783</v>
       </c>
       <c r="E2">
-        <v>0.8119608330726623</v>
+        <v>0.7249338030815125</v>
       </c>
       <c r="F2">
-        <v>0.8315466547012329</v>
+        <v>0.7461586594581604</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -985,19 +985,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.8360749292373657</v>
+        <v>0.7861067056655884</v>
       </c>
       <c r="C3">
-        <v>0.8929923725128174</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.8122667288780212</v>
+        <v>0.7459319829940796</v>
       </c>
       <c r="E3">
-        <v>0.80940682888031</v>
+        <v>0.7410250902175903</v>
       </c>
       <c r="F3">
-        <v>0.8324525213241577</v>
+        <v>0.773922860622406</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -15623,19 +15623,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.2210495817661285</v>
+        <v>0.25</v>
       </c>
       <c r="C2">
-        <v>0.2090187323093414</v>
+        <v>0.1965266764163971</v>
       </c>
       <c r="D2">
-        <v>0.2065007078647614</v>
+        <v>0.1869972348213196</v>
       </c>
       <c r="E2">
-        <v>0.2029902082681656</v>
+        <v>0.1812334507703781</v>
       </c>
       <c r="F2">
-        <v>0.2078866636753082</v>
+        <v>0.1865396648645401</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -15835,19 +15835,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2090187323093414</v>
+        <v>0.1965266764163971</v>
       </c>
       <c r="C3">
-        <v>0.2232480931282043</v>
+        <v>0.25</v>
       </c>
       <c r="D3">
-        <v>0.2030666822195053</v>
+        <v>0.1864829957485199</v>
       </c>
       <c r="E3">
-        <v>0.2023517072200775</v>
+        <v>0.1852562725543976</v>
       </c>
       <c r="F3">
-        <v>0.2081131303310394</v>
+        <v>0.1934807151556015</v>
       </c>
       <c r="G3">
         <v>0</v>

</xml_diff>

<commit_message>
update weighted average bert
</commit_message>
<xml_diff>
--- a/Output/Bert_output.xlsx
+++ b/Output/Bert_output.xlsx
@@ -773,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.8841983270645142</v>
       </c>
       <c r="C2">
-        <v>0.7861067056655884</v>
+        <v>0.8360749292373657</v>
       </c>
       <c r="D2">
-        <v>0.7479889392852783</v>
+        <v>0.8260028314590455</v>
       </c>
       <c r="E2">
-        <v>0.7249338030815125</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.7461586594581604</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -985,19 +985,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7861067056655884</v>
+        <v>0.8360749292373658</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.8929923725128175</v>
       </c>
       <c r="D3">
-        <v>0.7459319829940796</v>
+        <v>0.8122667288780213</v>
       </c>
       <c r="E3">
-        <v>0.7410250902175903</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.773922860622406</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -15623,19 +15623,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.2210495817661285</v>
       </c>
       <c r="C2">
-        <v>0.1965266764163971</v>
+        <v>0.2090187323093414</v>
       </c>
       <c r="D2">
-        <v>0.1869972348213196</v>
+        <v>0.2065007078647614</v>
       </c>
       <c r="E2">
-        <v>0.1812334507703781</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.1865396648645401</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -15835,19 +15835,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.1965266764163971</v>
+        <v>0.2090187323093415</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <v>0.2232480931282044</v>
       </c>
       <c r="D3">
-        <v>0.1864829957485199</v>
+        <v>0.2030666822195053</v>
       </c>
       <c r="E3">
-        <v>0.1852562725543976</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.1934807151556015</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>

</xml_diff>